<commit_message>
display all navigation elements in full screen
</commit_message>
<xml_diff>
--- a/testsuite_telnyx.xlsx
+++ b/testsuite_telnyx.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ЦяКнига" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Disk_D\TEST_QA\23.09.24_cypress_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6365B7-63A8-4AE9-9E63-BA381F4E20D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA803A1B-15F9-421A-8C40-C87BD8274842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65BB1E8D-FC1F-4BFB-92E2-9B728838C214}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{65BB1E8D-FC1F-4BFB-92E2-9B728838C214}"/>
   </bookViews>
   <sheets>
     <sheet name="Аркуш1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Expected Result</t>
   </si>
@@ -83,39 +83,6 @@
 9. Contact Us - посилання активне;
 10. Log In - посилання активне;
 11. Sign Up - посилання активне;</t>
-  </si>
-  <si>
-    <t>Елементи відображається правильно</t>
-  </si>
-  <si>
-    <t>Перевірка відображення:  
-1.Logo;  
-2. Products; 
-3. Solutions; 
-4. Pricing; 
-5. Why Telnyx; 
-6. Resources; 
-7. Developers; 
-8.Shop;
-9. Contact Us; 
-10. Log In; 
-11. Sign Up;</t>
-  </si>
-  <si>
-    <t>1. Відкрити браузер ;
-2. Перейти на https://telnyx.com; 
-3. Перевірити наявність відображення:
- 3. 1.Logo;
- 3. 2. Products;
- 3. 3. Solutions;
- 3. 4. Pricing;
- 3. 5. Why Telnyx;
- 3. 6. Resources;
- 3. 7. Developers;
- 3. 8.Shop;
- 3.9. Contact Us;
- 3.10. Log In;
- 3. 11. Sign Up;</t>
   </si>
   <si>
     <t>1. Відкрити браузер ;
@@ -134,9 +101,6 @@
  3. 11. Sign Up;</t>
   </si>
   <si>
-    <t>Check Display of Navigation Panel Elements</t>
-  </si>
-  <si>
     <t>Check Activity of Links on Navigation Panel</t>
   </si>
   <si>
@@ -158,22 +122,6 @@
   </si>
   <si>
     <t>Elements are displayed correctly</t>
-  </si>
-  <si>
-    <t>1.Open browser ;
-2. Go to https://telnyx.com; 
-3. Check for display presence:
- 3. 1.Logo;
- 3. 2. Products;
- 3. 3. Solutions;
- 3. 4. Pricing;
- 3. 5. Why Telnyx;
- 3. 6. Resources;
- 3. 7. Developers;
- 3. 8.Shop;
- 3.9. Contact Us;
- 3.10. Log In;
- 3. 11. Sign Up;</t>
   </si>
   <si>
     <t>Check activity of elements: 
@@ -260,6 +208,67 @@
     <t>Перевірка посилань в підменю 'Products'</t>
   </si>
   <si>
+    <t>Checking the links in the ‘Products’ submenu</t>
+  </si>
+  <si>
+    <t>User is on the main page https://telnyx.com in the ‘Products’ submenu</t>
+  </si>
+  <si>
+    <t>Checking the activity of elements:
+1. SMS API;
+2. IoT SIM Card; 
+3. Inference; 
+4. Global Numbers; 
+5. Voice API; 
+6. Cloud Storage; 
+7. See all products; 
+8.  SIP Trunking; 
+9. Microsoft Teams; 
+10.  WebRTC;</t>
+  </si>
+  <si>
+    <t>Links are active:
+1. SMS API;
+2. IoT SIM Card; 
+3. Inference; 
+4. Global Numbers; 
+5. Voice API; 
+6. Cloud Storage; 
+7. See all products; 
+8.  SIP Trunking; 
+9. Microsoft Teams; 
+10.  WebRTC;</t>
+  </si>
+  <si>
+    <t>Перевірка активності елементів: 
+1. SMS API;
+2. IoT SIM Card; 
+3. Inference; 
+4. Global Numbers; 
+5. Voice API; 
+6. Cloud Storage; 
+7. See all products; 
+8.  SIP Trunking; 
+9. Microsoft Teams; 
+10.  WebRTC;</t>
+  </si>
+  <si>
+    <t>1. Відкрити браузер ;
+2. Перейти на https://telnyx.com; 
+3. Перейти в підменю 'Products';
+4. Перевірити активність посилань:
+ 4.1. SMS API;
+ 4.2. IoT SIM Card; 
+ 4.3. Inference; 
+ 4.4. Global Numbers; 
+ 4.5. Voice API; 
+ 4.6. Cloud Storage; 
+ 4.7. See all products; 
+ 4.8.  SIP Trunking; 
+ 4.9. Microsoft Teams; 
+ 4.10.  WebRTC;</t>
+  </si>
+  <si>
     <t>Посилання активні:
 1. SMS API;
 2. IoT SIM Card; 
@@ -273,33 +282,111 @@
 10.  WebRTC;</t>
   </si>
   <si>
-    <t>Перевірка активності елементів: 
-1. SMS API;
-2. IoT SIM Card; 
-3. Inference; 
-4. Global Numbers; 
-5. Voice API; 
-6. Cloud Storage; 
-7. See all products; 
-8.  SIP Trunking; 
-9. Microsoft Teams; 
-10.  WebRTC;</t>
-  </si>
-  <si>
-    <t>1. Відкрити браузер ;
-2. Перейти на https://telnyx.com; 
-3. Перейти в підменю 'Products'
-4. Перевірити активність посилань:
- 4.1. SMS API;
- 4.2. IoT SIM Card; 
- 4.3. Inference; 
- 4.4. Global Numbers; 
- 4.5. Voice API; 
- 4.6. Cloud Storage; 
- 4.7. See all products; 
- 4.8.  SIP Trunking; 
- 4.9. Microsoft Teams; 
- 4.10.  WebRTC;</t>
+    <t>1. Open the browser;
+2. Go to https://telnyx.com;
+3. Navigate to the ‘Products’ submenu;
+4. Check the activity of the links: 
+ 4.1. SMS API ;
+ 4.2. IoT SIM Card ;
+ 4.3. Inference ;
+ 4.4. Global Numbers ;
+ 4.5. Voice API;
+ 4.6. Cloud Storage;
+ 4.7. See all products;
+ 4.8. SIP Trunking;
+ 4.9. Microsoft Teams;
+ 4.10. WebRTC</t>
+  </si>
+  <si>
+    <t>Check Display of Navigation Panel Elements (Full Screen)</t>
+  </si>
+  <si>
+    <t>Check Display of Navigation Panel Elements (non-Full Screen)</t>
+  </si>
+  <si>
+    <t>Перевірка відображення елементів навігаційної панелі  (Full Screen)</t>
+  </si>
+  <si>
+    <t>Елементи відображається правильно.</t>
+  </si>
+  <si>
+    <t>Перевірка відображення:  
+1.Logo;  
+2. Products; 
+3. Solutions; 
+4. Pricing; 
+5. Why Telnyx; 
+6. Resources; 
+7. Developers; 
+8.Shop;
+9. Contact Us; 
+10. Log In; 
+11. Sign Up;</t>
+  </si>
+  <si>
+    <t>1. Користувач знаходиться на головній сторінці https://telnyx.com/.
+2. Full-Screen 1920x1080</t>
+  </si>
+  <si>
+    <t>1. Користувач знаходиться на головній сторінці https://telnyx.com/.
+2. Full-Screen 12800x800</t>
+  </si>
+  <si>
+    <t>Check display of: 
+1.Logo;  
+2. Products; 
+3. Solutions; 
+4. Pricing; 
+5. Why Telnyx; 
+6. Resources; 
+7. Developers; 
+8.Shop;
+9. Contact Us; 
+10. Log In; 
+11. Sign Up;</t>
+  </si>
+  <si>
+    <t>1. User is on the main page  https://telnyx.com/.
+2. Full-Screen 1920x1080.</t>
+  </si>
+  <si>
+    <t>Elements are displayed correctly.</t>
+  </si>
+  <si>
+    <t>1. Відкрити браузер.
+2. Перейти на https://telnyx.com/.
+3. Встановити розштрення екрана 1920 х 1080 px.
+4. Перевірити наявність відображення header.
+5.Якщо header відображається, перевірити наявність відображення навігаційної панелі:
+ 5. 1.Logo;
+ 5. 2. Products;
+ 5. 3. Solutions;
+ 5. 4. Pricing;
+ 5. 5. Why Telnyx;
+ 5. 6. Resources;
+ 5. 7. Developers;
+ 5. 8.Shop;
+ 5.9. Contact Us;
+ 5.10. Log In;
+ 5. 11. Sign Up;</t>
+  </si>
+  <si>
+    <t>1. Open the browser.
+2. Go to https://telnyx.com/.
+3. Check for the display of the header.
+4. Set the screen resolution to 1920 x 1080 px.
+5. If the header is displayed, check for the display of the navigation panel elements: 
+ 5. 1.Logo;
+ 5. 2. Products;
+ 5. 3. Solutions;
+ 5. 4. Pricing;
+ 5. 5. Why Telnyx;
+ 5. 6. Resources;
+ 5. 7. Developers;
+ 5. 8.Shop;
+ 5.9. Contact Us;
+ 5.10. Log In;
+ 5. 11. Sign Up;</t>
   </si>
 </sst>
 </file>
@@ -694,20 +781,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3249E3F-1463-465D-89AE-258F32BB99DA}">
-  <dimension ref="A1:F7"/>
+  <sheetPr codeName="Аркуш1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
-    <col min="5" max="5" width="37.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.77734375" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="5" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="39.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -730,84 +817,98 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="216" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -818,20 +919,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BEDADF3-8687-434D-A3C7-F1B67BBC9909}">
-  <dimension ref="A1:F6"/>
+  <sheetPr codeName="Аркуш2"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.44140625" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.44140625" customWidth="1"/>
-    <col min="5" max="5" width="37.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="37.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -854,67 +956,107 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
display all navigation elements in non-full screen
</commit_message>
<xml_diff>
--- a/testsuite_telnyx.xlsx
+++ b/testsuite_telnyx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Disk_D\TEST_QA\23.09.24_cypress_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3FE112-F7B7-4158-AC52-F2D61BC07FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7937F022-617E-4B19-B167-C8DDC23FDF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{65BB1E8D-FC1F-4BFB-92E2-9B728838C214}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>Expected Result</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Перевірка активності посилань на навігаційній панелі</t>
-  </si>
-  <si>
-    <t>Перевірка відображення елементів навігаційної панелі</t>
   </si>
   <si>
     <t>Користувач знаходиться на головній сторінці https://telnyx.com</t>
@@ -104,23 +101,6 @@
     <t>Check Activity of Links on Navigation Panel</t>
   </si>
   <si>
-    <t>Check display of:  
-1.Logo;  
-2. Products; 
-3. Solutions; 
-4. Pricing; 
-5. Why Telnyx; 
-6. Resources; 
-7. Developers; 
-8.Shop;
-9. Contact Us; 
-10. Log In; 
-11. Sign Up;</t>
-  </si>
-  <si>
-    <t>User is on the main page  https://telnyx.com</t>
-  </si>
-  <si>
     <t>Elements are displayed correctly</t>
   </si>
   <si>
@@ -345,9 +325,20 @@
     <t>Elements are displayed correctly.</t>
   </si>
   <si>
+    <t>1. Користувач знаходиться на головній сторінці https://telnyx.com/.
+2. Full-Screen 1280x800.</t>
+  </si>
+  <si>
+    <t>1. Користувач знаходиться на головній сторінці https://telnyx.com/.
+2. Full-Screen 1920x1080.</t>
+  </si>
+  <si>
+    <t>Перевірка відображення елементів навігаційної панелі (non-Full Screen)</t>
+  </si>
+  <si>
     <t>1. Відкрити браузер.
-2. Перейти на https://telnyx.com/.
-3. Встановити розштрення екрана 1920 х 1080 px.
+2. Встановити розштрення екрана 1920 х 1080 px.
+3. Перейти на https://telnyx.com/.
 4. Перевірити наявність відображення header.
 5.Якщо header відображається, перевірити наявність відображення навігаційної панелі:
  5. 1.Logo;
@@ -363,10 +354,44 @@
  5. 11. Sign Up;</t>
   </si>
   <si>
+    <t>Перевірка відображення:  
+1. Logo.
+2. Sign Up.
+3. Main menu.
+ 3.1. Products; 
+ 3.2. Solutions; 
+ 3.3. Pricing; 
+ 3.4. Why Telnyx; 
+ 3.5. Resources; 
+ 3.6. Developers; 
+ 3.7.Shop;
+ 3.8. Contact Us; 
+ 3.9. Log In;</t>
+  </si>
+  <si>
+    <t>Check display of:  
+1. Logo.
+2. Sign Up.
+3. Main menu.
+ 3.1. Products; 
+ 3.2. Solutions; 
+ 3.3. Pricing; 
+ 3.4. Why Telnyx; 
+ 3.5. Resources; 
+ 3.6. Developers; 
+ 3.7.Shop;
+ 3.8. Contact Us; 
+ 3.9. Log In;</t>
+  </si>
+  <si>
+    <t>1. User is on the main page  https://telnyx.com.
+2. Full-Screen 1280x800.</t>
+  </si>
+  <si>
     <t>1. Open the browser.
-2. Go to https://telnyx.com/.
-3. Check for the display of the header.
-4. Set the screen resolution to 1920 x 1080 px.
+2. Set the screen resolution to 1920 x 1080 px
+3. Go to https://telnyx.com/..
+4. Check for the display of the header.
 5. If the header is displayed, check for the display of the navigation panel elements: 
  5. 1.Logo;
  5. 2. Products;
@@ -381,12 +406,45 @@
  5. 11. Sign Up;</t>
   </si>
   <si>
-    <t>1. Користувач знаходиться на головній сторінці https://telnyx.com/.
-2. Full-Screen 1280x800.</t>
-  </si>
-  <si>
-    <t>1. Користувач знаходиться на головній сторінці https://telnyx.com/.
-2. Full-Screen 1920x1080.</t>
+    <t>1. Відкрити браузер.
+2. Встановити розширення екрана 1280 х 800 px.
+3. Перейти на https://telnyx.com/ .
+4. Перевірити наявність відображення header.
+5. Якщо header відображається, перевірити наявність відображення навігаційної панелі:
+ 5.1. Logo.
+ 5.2. Sign Up.
+ 5.3. Main menu. Якщо Main menu відображається, перевірити наявність відображення елеменетів в підменю :
+  5.3.1. Products; 
+  5.3.2. Solutions; 
+  5.3.3. Pricing; 
+  5.3.4. Why Telnyx; 
+  5.3.5. Resources; 
+  5.3.6. Developers; 
+  5.3.7.Shop;
+  5.3.8. Contact Us; 
+  5.3.9. Log In;</t>
+  </si>
+  <si>
+    <t>1. Open the browser.
+2. Set the screen resolution to 1280 x 800 px
+3. Go to https://telnyx.com/..
+4. Check for the display of the header.
+5. If the header is displayed, check for the display of the navigation panel elements: 
+ 5.1. Logo 
+ 5.2. Sign Up
+ 5.3. Main menu. If the Main menu is displayed, check the display of submenu elements: 
+  5.3.1. Products
+  5.3.2. Solutions
+  5.3.3. Pricing 
+  5.3.4. Why Telnyx 
+  5.3.5. Resources
+  5.3.6. Developers
+  5.3.7. Shop
+  5.3.8. Contact Us
+  5.3.9. Log In</t>
+  </si>
+  <si>
+    <t>05</t>
   </si>
 </sst>
 </file>
@@ -784,9 +842,7 @@
   <sheetPr codeName="Аркуш1"/>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -817,39 +873,45 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="361.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -859,36 +921,36 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -896,7 +958,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -905,10 +967,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -922,9 +984,7 @@
   <sheetPr codeName="Аркуш2"/>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -932,8 +992,8 @@
     <col min="2" max="2" width="21.44140625" customWidth="1"/>
     <col min="3" max="3" width="21.6640625" customWidth="1"/>
     <col min="4" max="4" width="21.44140625" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="6" width="37.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" customWidth="1"/>
+    <col min="6" max="6" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -956,82 +1016,84 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="375" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="316.8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1039,7 +1101,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1048,10 +1110,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add README, change package.json, cypress.config, POM
</commit_message>
<xml_diff>
--- a/testsuite_telnyx.xlsx
+++ b/testsuite_telnyx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ЦяКнига" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Disk_D\TEST_QA\23.09.24_cypress_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Disk_D\TEST_QA\23.09.24_cypress_test_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42987EB1-2E98-4CE2-A143-20C609330CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208FD070-E64E-4A98-9BA6-F73B4D3EB99E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{65BB1E8D-FC1F-4BFB-92E2-9B728838C214}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{65BB1E8D-FC1F-4BFB-92E2-9B728838C214}"/>
   </bookViews>
   <sheets>
     <sheet name="ukr" sheetId="1" r:id="rId1"/>
@@ -166,24 +166,6 @@
  3.9. Log In;</t>
   </si>
   <si>
-    <t>1. Open the browser.
-2. Set the screen resolution to 1920 x 1080 px
-3. Go to https://telnyx.com/..
-4. Check for the display of the header.
-5. If the header is displayed, check for the display of the navigation panel elements: 
- 5. 1.Logo;
- 5. 2. Products;
- 5. 3. Solutions;
- 5. 4. Pricing;
- 5. 5. Why Telnyx;
- 5. 6. Resources;
- 5. 7. Developers;
- 5. 8.Shop;
- 5.9. Contact Us;
- 5.10. Log In;
- 5. 11. Sign Up;</t>
-  </si>
-  <si>
     <t>1. Відкрити браузер.
 2. Встановити розширення екрана 1280 х 800 px.
 3. Перейти на https://telnyx.com/ .
@@ -594,6 +576,24 @@
 7. Verify the page that opens.
 8. Follow the link to the social network ‘facebook.com’.
 9. Verify the page that opens.</t>
+  </si>
+  <si>
+    <t>1. Open the browser.
+2. Set the screen resolution to 1920 x 1080 px
+3. Go to https://telnyx.com/.
+4. Check for the display of the header.
+5. If the header is displayed, check for the display of the navigation panel elements: 
+ 5. 1.Logo;
+ 5. 2. Products;
+ 5. 3. Solutions;
+ 5. 4. Pricing;
+ 5. 5. Why Telnyx;
+ 5. 6. Resources;
+ 5. 7. Developers;
+ 5. 8.Shop;
+ 5.9. Contact Us;
+ 5.10. Log In;
+ 5. 11. Sign Up;</t>
   </si>
 </sst>
 </file>
@@ -1003,9 +1003,9 @@
   <sheetPr codeName="Аркуш1"/>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,7 +1070,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1078,17 +1078,17 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
@@ -1096,142 +1096,142 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="153" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="77.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" s="5"/>
     </row>
@@ -1254,9 +1254,9 @@
   <sheetPr codeName="Аркуш2"/>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,7 +1289,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="214.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1322,7 +1322,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="67.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -1330,17 +1330,17 @@
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1348,119 +1348,119 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="13" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>

</xml_diff>